<commit_message>
Added button and webBrowser
Start not use Abbreviations for naming fields and variables
</commit_message>
<xml_diff>
--- a/noteDuringDevelopment.xlsx
+++ b/noteDuringDevelopment.xlsx
@@ -79,17 +79,17 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -146,6 +146,66 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1897380</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="358140" y="3901440"/>
+          <a:ext cx="1897380" cy="213360"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -420,7 +480,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,110 +490,110 @@
     <col min="3" max="3" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="1"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>